<commit_message>
-Telas editar matricula 1 e 2 adicionadas; -Adicionado funcionalidade de excluir matricula; -Funcionalidade de editar matricula em desenvolvimento.
</commit_message>
<xml_diff>
--- a/base_dados_alunos.xlsx
+++ b/base_dados_alunos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4068,7 +4068,6 @@
           <t>NÃO</t>
         </is>
       </c>
-      <c r="AW14" t="inlineStr"/>
       <c r="AX14" t="inlineStr">
         <is>
           <t>5</t>
@@ -4085,6 +4084,1791 @@
         </is>
       </c>
       <c r="BA14" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mathbr</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>666</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>pa</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>minicip</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>munici</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>endereco</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>comp</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>bairro</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>email@email.com</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>pai</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>mãe</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>escola</t>
+        </is>
+      </c>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ15" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR15" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS15" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT15" t="inlineStr">
+        <is>
+          <t>04 - Escola Particular</t>
+        </is>
+      </c>
+      <c r="AU15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>linao</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>uf</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nome cart</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>carto</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>pc</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>uf</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>pai</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>mae</t>
+        </is>
+      </c>
+      <c r="AM16" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO16" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ16" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR16" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS16" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT16" t="inlineStr">
+        <is>
+          <t>03 - Escola Estadual</t>
+        </is>
+      </c>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Creo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>UF</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO17" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ17" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR17" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS17" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT17" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ18" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR18" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS18" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT18" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO19" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ19" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR19" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS19" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT19" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA19" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ20" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR20" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS20" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT20" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AX20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AY20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA20" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>22070053</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Leonardo Bernardes</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>endereco</t>
+        </is>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH21" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>a@a.a</t>
+        </is>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>Pai</t>
+        </is>
+      </c>
+      <c r="AL21" t="inlineStr">
+        <is>
+          <t>Mãe</t>
+        </is>
+      </c>
+      <c r="AM21" t="inlineStr">
+        <is>
+          <t>escola</t>
+        </is>
+      </c>
+      <c r="AN21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO21" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ21" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR21" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS21" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT21" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr"/>
+      <c r="AX21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AY21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA21" t="inlineStr">
         <is>
           <t>2000-01-01</t>
         </is>

</xml_diff>

<commit_message>
-Adicionado função de editar alunos; -Adicionado função de excluir alunos;
</commit_message>
<xml_diff>
--- a/base_dados_alunos.xlsx
+++ b/base_dados_alunos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA24"/>
+  <dimension ref="A1:BA25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6623,10 +6623,262 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AX24" t="inlineStr"/>
-      <c r="AY24" t="inlineStr"/>
-      <c r="AZ24" t="inlineStr"/>
       <c r="BA24" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AD25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AL25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AM25" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AN25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO25" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ25" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR25" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS25" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT25" t="inlineStr">
+        <is>
+          <t>02 - Escola Municipal</t>
+        </is>
+      </c>
+      <c r="AU25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr"/>
+      <c r="AY25" t="inlineStr"/>
+      <c r="AZ25" t="inlineStr"/>
+      <c r="BA25" t="inlineStr">
         <is>
           <t>2000-01-01</t>
         </is>

</xml_diff>

<commit_message>
Correção de bug ao excluir alunos.
</commit_message>
<xml_diff>
--- a/base_dados_alunos.xlsx
+++ b/base_dados_alunos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA25"/>
+  <dimension ref="A1:BA28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6875,10 +6875,791 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AX25" t="inlineStr"/>
-      <c r="AY25" t="inlineStr"/>
-      <c r="AZ25" t="inlineStr"/>
       <c r="BA25" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH26" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO26" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ26" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AR26" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS26" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT26" t="inlineStr">
+        <is>
+          <t>01 - Do Lar</t>
+        </is>
+      </c>
+      <c r="AU26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>aluno 1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH27" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+      <c r="AI27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>pai</t>
+        </is>
+      </c>
+      <c r="AL27" t="inlineStr">
+        <is>
+          <t>mae</t>
+        </is>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO27" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ27" t="inlineStr">
+        <is>
+          <t>19/1/2000</t>
+        </is>
+      </c>
+      <c r="AR27" t="inlineStr">
+        <is>
+          <t>Tempo Integral</t>
+        </is>
+      </c>
+      <c r="AS27" t="inlineStr">
+        <is>
+          <t>03. Maternal I</t>
+        </is>
+      </c>
+      <c r="AT27" t="inlineStr">
+        <is>
+          <t>04 - Escola Particular</t>
+        </is>
+      </c>
+      <c r="AU27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AX27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AY27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AZ27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="BA27" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>213</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>aa</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>Rural</t>
+        </is>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AM28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AN28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO28" t="inlineStr">
+        <is>
+          <t>1/1/2000</t>
+        </is>
+      </c>
+      <c r="AP28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AQ28" t="inlineStr">
+        <is>
+          <t>20/1/2000</t>
+        </is>
+      </c>
+      <c r="AR28" t="inlineStr">
+        <is>
+          <t>Tempo Integral</t>
+        </is>
+      </c>
+      <c r="AS28" t="inlineStr">
+        <is>
+          <t>08. Ciclo I - 2° Ano</t>
+        </is>
+      </c>
+      <c r="AT28" t="inlineStr">
+        <is>
+          <t>06 - Escola Comunitária</t>
+        </is>
+      </c>
+      <c r="AU28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AV28" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX28" t="inlineStr"/>
+      <c r="AY28" t="inlineStr"/>
+      <c r="AZ28" t="inlineStr"/>
+      <c r="BA28" t="inlineStr">
         <is>
           <t>2000-01-01</t>
         </is>

</xml_diff>

<commit_message>
atualizando a IU e a segurança de usuário
</commit_message>
<xml_diff>
--- a/base_dados_alunos.xlsx
+++ b/base_dados_alunos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA7"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2244,7 +2244,6 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="inlineStr">
         <is>
           <t>2131</t>
@@ -2263,6 +2262,273 @@
       <c r="BA7" t="inlineStr">
         <is>
           <t>2000-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>29129</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>aluno teste</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Branca</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Belem</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Belem</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2000-01-05</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>11111111111</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>NÃO</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>Rua Teste</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>Teste 123</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>01290129</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>teste@gmail.com</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="AQ8" t="inlineStr">
+        <is>
+          <t>29/1/2024</t>
+        </is>
+      </c>
+      <c r="AR8" t="inlineStr">
+        <is>
+          <t>Manhã</t>
+        </is>
+      </c>
+      <c r="AS8" t="inlineStr">
+        <is>
+          <t>01. Berçário I</t>
+        </is>
+      </c>
+      <c r="AT8" t="inlineStr">
+        <is>
+          <t>03 - Escola Estadual</t>
+        </is>
+      </c>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>2000-01-05</t>
         </is>
       </c>
     </row>

</xml_diff>